<commit_message>
Converting from Map Editor to Map Inspector
Moving away from a separate window/editor for the map controls, moving
it to be a part of the inspector. Painting the textures on the tiles is
also implemented.
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Description</t>
   </si>
@@ -35,9 +35,6 @@
     </r>
   </si>
   <si>
-    <t>prevent drag-selecting tiles when they are 'locked'</t>
-  </si>
-  <si>
     <t>Implement tile-texture 'paint' tool</t>
   </si>
   <si>
@@ -60,6 +57,27 @@
   </si>
   <si>
     <t>Add visual indicator for the selected tile in the Map Editor</t>
+  </si>
+  <si>
+    <t>prevent multi-selecting tiles when they are 'locked'</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>when the map is selected you cannot select anything, so it's half fixed.</t>
+  </si>
+  <si>
+    <t>Remove textures from the Map Editor tileset</t>
+  </si>
+  <si>
+    <t>was done for the Editor window, need to reimplement for the inspector.</t>
+  </si>
+  <si>
+    <t>Drag to create regions on the map</t>
+  </si>
+  <si>
+    <t>Modify map to have transform data for width/height</t>
   </si>
 </sst>
 </file>
@@ -91,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +119,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -181,9 +205,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,16 +512,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M35"/>
+  <dimension ref="B2:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="97" customWidth="1"/>
+    <col min="4" max="4" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -504,7 +532,9 @@
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -520,7 +550,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -538,7 +568,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -552,13 +582,15 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+      <c r="B5" s="15">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -570,11 +602,11 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>10</v>
+      <c r="C6" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -588,11 +620,11 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="10">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
+      <c r="C7" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -607,12 +639,12 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -624,13 +656,15 @@
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7"/>
+      <c r="B9" s="12">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -646,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -660,9 +694,13 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -687,8 +725,12 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -701,8 +743,12 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -715,8 +761,12 @@
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="3">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -883,12 +933,8 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="3">
-        <v>4</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -998,22 +1044,8 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-    </row>
   </sheetData>
-  <sortState ref="B3:C10">
+  <sortState ref="B3:D11">
     <sortCondition descending="1" ref="B3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Set Tile Pathing Mode
- The map inspector can now 'paint' onto the tiles a pathing mode.
- While painting, a filter is drawn over each tile to indicate which
mode it currently has.
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -77,13 +77,13 @@
     <t>Modify map to have transform data for width/height</t>
   </si>
   <si>
-    <t>Create pathing window (buttons to define new regions/points)</t>
-  </si>
-  <si>
     <t>fix material leak when painting textures onto map tiles</t>
   </si>
   <si>
     <t>looks alright, could use a little work. Very low priority</t>
+  </si>
+  <si>
+    <t>Create pathing inspector (buttons to define new regions/points)</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -685,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -720,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
@@ -766,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>

</xml_diff>

<commit_message>
Messenger-Based Event System Implemented
Implemented a skeleton for the finished event system. Objects simply
register with a static 'Messenger' class for events the fire and listen
to. Defining often-used base events will come next.
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Description</t>
   </si>
@@ -94,12 +94,39 @@
   <si>
     <t>Dynamic terrain manipulation + path regeneration</t>
   </si>
+  <si>
+    <t>Build Editor extension for Event system.</t>
+  </si>
+  <si>
+    <t>Begin defining types of events</t>
+  </si>
+  <si>
+    <t>Begin defining types of actions</t>
+  </si>
+  <si>
+    <t>Region Editor</t>
+  </si>
+  <si>
+    <t>Ability to define regions through the editor.</t>
+  </si>
+  <si>
+    <t>Implement event system skeleton -- how it will work at all</t>
+  </si>
+  <si>
+    <t>done, using a global messenger system</t>
+  </si>
+  <si>
+    <t>Ensure events wired in the editor are serialized and stored for the objects.</t>
+  </si>
+  <si>
+    <t>http://answers.unity3d.com/questions/526361/saving-data-made-using-the-editor.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +146,14 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,10 +235,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -225,8 +261,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M37"/>
+  <dimension ref="B2:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,8 +919,12 @@
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -894,8 +937,12 @@
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -908,8 +955,12 @@
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -922,9 +973,15 @@
       <c r="M23" s="3"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="B24" s="7">
+        <v>5</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -936,9 +993,15 @@
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -951,7 +1014,7 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -964,12 +1027,8 @@
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>2</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -983,7 +1042,7 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -997,7 +1056,7 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1010,8 +1069,12 @@
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1024,8 +1087,12 @@
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
+      <c r="B31" s="2">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1039,7 +1106,7 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1053,7 +1120,7 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="5"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1067,7 +1134,7 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1081,7 +1148,7 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1095,7 +1162,7 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1121,11 +1188,186 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>2</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+    </row>
   </sheetData>
   <sortState ref="B14:C17">
     <sortCondition descending="1" ref="B14"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="D25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>